<commit_message>
add keys in config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indra\OneDrive\Desktop\Current_Batch\IA.001.InvoiceProcessing_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A38D763-B36A-4193-A3B7-FCF4C4C78441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D9536C-F244-451F-A6F1-AD75A6AFF898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>SharedFolder</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -646,7 +649,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>